<commit_message>
Add Requirements and Readme
</commit_message>
<xml_diff>
--- a/data/sanads.vn.xlsx
+++ b/data/sanads.vn.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D597"/>
+  <dimension ref="A1:D757"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14397,6 +14397,3768 @@
         </is>
       </c>
     </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61561095482591</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Minh Anh Tran</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>Thiết kế Logo - Nhận diện thương hiệu
+Thiết kế Website - LDPage
+Đăng ký bảo hộ thương hiệu
+0978060082</t>
+        </is>
+      </c>
+      <c r="D598" t="inlineStr">
+        <is>
+          <t>0978060082</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/nguyen.minh.hang.146432</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Nguyễn Minh Hằng</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>Tư vấn nguồn hàng và vận chuyển Trung Quốc,Việt Nam đi ĐNA, Mỹ, UAE,…
+Liên hệ: 0912 957 718</t>
+        </is>
+      </c>
+      <c r="D599" t="inlineStr">
+        <is>
+          <t>0912957718</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/trung.cule.93</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Nguyễn Đình Trung</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>👉Tăng sub mọi nền tảng MXH, mở khóa FB 🔰
+👉Chạy QC FB, Tiktok 💵
+☎️ Zalo :0862.265.345✅</t>
+        </is>
+      </c>
+      <c r="D600" t="inlineStr">
+        <is>
+          <t>0862265345</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/ngocminhvmu</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Ngọc Minh</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>Dr.Ngọc Minh - Đào tạo MD Codes - 📞 0973731319 (5 Cơ Sở)</t>
+        </is>
+      </c>
+      <c r="D601" t="inlineStr">
+        <is>
+          <t>0973731319</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/duoclieutot.vn</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Ngô Quốc Hưng</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>Founder: KOVI Group. Founder: Cao An Xoa Agan. Phone: 09.3449.3449</t>
+        </is>
+      </c>
+      <c r="D602" t="inlineStr">
+        <is>
+          <t>0934493449</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/maiphuongjobup.hr</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Mai Phương</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>Contact for work: Zalo 0868213097 or
+Email: mphuongnt.jobup@gmail.com</t>
+        </is>
+      </c>
+      <c r="D603" t="inlineStr">
+        <is>
+          <t>0868213097</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100094627219112</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Đức Quân</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>👑𝐜𝐡𝐮𝐲Ê𝐧 𝐪𝐮Ầ𝐧 Á𝐨 𝐪𝐮Ả𝐧𝐠 𝐜𝐡Â𝐮 𝐥𝐮𝐱𝐮𝐫𝐲👑. ☎️ 0339580785. Nhận ship toàn quốc❤️</t>
+        </is>
+      </c>
+      <c r="D604" t="inlineStr">
+        <is>
+          <t>0339580785</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/minhkhoibangbom</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Thu Trang</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>Vận chuyển Trung - Việt và ĐNA
+Cung cấp dịch vụ Fulfillment ĐNA
+☎️ Zalo: 098.974.3578 - Ms. Thu Trang</t>
+        </is>
+      </c>
+      <c r="D605" t="inlineStr">
+        <is>
+          <t>0989743578</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/thanhson.bui.104</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Bùi Thanh Sơn</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>Work - edu:
+0949.65.61.62
+email: SBCinex@gmail.com</t>
+        </is>
+      </c>
+      <c r="D606" t="inlineStr">
+        <is>
+          <t>0949656162</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/cuong.truong.313</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Trương Quang Cường</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>🇻🇳Mua Bán - Cầm Cố Sim Số Đẹp - Sĩ Lẻ Iphone ☎️: - 037.48.45678 🔥
+GDH Full Hà Tĩnh</t>
+        </is>
+      </c>
+      <c r="D607" t="inlineStr">
+        <is>
+          <t>0374845678</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/AnhQuanPlastic</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Anh Quann</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>Chuyên sản xuất đồ nhựa dùng 1 lần
+Đt/Zalo 0936259892</t>
+        </is>
+      </c>
+      <c r="D608" t="inlineStr">
+        <is>
+          <t>0936259892</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/SangTickXanh</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Nguyễn Tấn Sang</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>Tăng Tương Tác-Mở Khóa-Bảo Mật
+Chạy Quảng Cáo Facebook-TikTok-Google
+☎️Hotline/Zalo: 0365 456 918☎️</t>
+        </is>
+      </c>
+      <c r="D609" t="inlineStr">
+        <is>
+          <t>0365456918</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/giangsimso</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Đỗ Trường Giang</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>Call/Sms/Zalo/Viber 0962.86.6688 KHOSIMONLINE.COM</t>
+        </is>
+      </c>
+      <c r="D610" t="inlineStr">
+        <is>
+          <t>0962866688</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61563134742441</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Phạm Thảo Linh</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>UY TÍN - CHẤT LƯỢNG - NHANH CHÓNG
+Chuyên Order - Vận chuyển - OEM
+TQ ➡️ ĐNA
+☎️ ZALO 0333 209 396</t>
+        </is>
+      </c>
+      <c r="D611" t="inlineStr">
+        <is>
+          <t>0333209396</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/pijkay2803</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Lê Gia Bảo</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>FaceBook-TikTok
+Hỗ Trợ Nhà bán Hàng
+zalo:0396903234
+MB:2222229996666
+PHONE:0522222755</t>
+        </is>
+      </c>
+      <c r="D612" t="inlineStr">
+        <is>
+          <t>0396903234, 0522222755</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/PAD212</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Phạm Dũng</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>sɪᴍ số đẹᴘ - sᴛᴋ ʙᴀɴᴋ ᴠɪᴘ
+ᴛᴋɢʀ &amp; ᴍxʜ
+𝓱𝓸𝓽𝓵𝓲𝓷𝓮 : 0966.586.779</t>
+        </is>
+      </c>
+      <c r="D613" t="inlineStr">
+        <is>
+          <t>0966586779</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/binh.nguyenlong.982</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Nguyễn Long Bình</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>Contact For Work : 036.846.0114</t>
+        </is>
+      </c>
+      <c r="D614" t="inlineStr">
+        <is>
+          <t>0368460114</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100092618826369</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Vũ Chiến</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>Mr Chiến : Chuyên cung cấp BĐS để ở và đầu tư khu vực Hà Đông - Chương Mỹ
+Hotline : 0824861996</t>
+        </is>
+      </c>
+      <c r="D615" t="inlineStr">
+        <is>
+          <t>0824861996</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/Tu799799</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Tú Bình Dương</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>Giao Sim nhanh loanh quanh Thủ Dầu Một Hotline ☎ 0899799799</t>
+        </is>
+      </c>
+      <c r="D616" t="inlineStr">
+        <is>
+          <t>0899799799</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/tuo.lo.79</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Lê Minh Tưởng ✅</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>XỬ LÍ CÁC VẤN ĐỀ Về FACEBOOK
+Xoá tài khoản fb tiktok - unlock fb
+zalo 0376599885</t>
+        </is>
+      </c>
+      <c r="D617" t="inlineStr">
+        <is>
+          <t>0376599885</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/minhquannet2</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Trần Văn Quân</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>LẮP ĐẶT PHÒNG NET - THANH LÝ PHÒNG NET - MÁY BỘ CHƠI GAME - LAPTOP GAMING -VE CHAI PC - 0911 242 242</t>
+        </is>
+      </c>
+      <c r="D618" t="inlineStr">
+        <is>
+          <t>0911242242</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/minhducmktfb</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Tuấn Trần</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>CHẠY QUẢNG CÁO LIVE + MESS + CĐ..
+Nhận Tất Cả Các Dịch Vụ FACEBOOK
+Liên hệ SĐT và ZALO:
+0373641347</t>
+        </is>
+      </c>
+      <c r="D619" t="inlineStr">
+        <is>
+          <t>0373641347</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/ngoc.tu.963871</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Nguyễn Ngọc Tú</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>ACTOR - PRODUCE
+For work : 0364354113
+Nguyenngoctu7299@gmail.com</t>
+        </is>
+      </c>
+      <c r="D620" t="inlineStr">
+        <is>
+          <t>0364354113</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/lequyfanpage12</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Lê Quý</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>Mua Bán FanPage
+Hỗ trợ &amp; xử lý mọi vấn đề về Facebook-Instargram-TikTok
+Contact/Zalo :☎️086.549.4473</t>
+        </is>
+      </c>
+      <c r="D621" t="inlineStr">
+        <is>
+          <t>0865494473</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/kim.nhan.104855</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Kim Thoa</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>TƯ VẤN KHÓA HỌC ONLINE NHIỆT TÌNH UY TÍN CHẤT LƯỢNG . LIÊN HỆ ZALO : 0971781063 ĐỂ MÌNH TƯ VẤN NHA</t>
+        </is>
+      </c>
+      <c r="D622" t="inlineStr">
+        <is>
+          <t>0971781063</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/quangminh.tran.509511</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Trần Quang Minh</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>CẤP BM2500 - TKQC chính chủ
+Phí chỉ từ 3% cân VPCS
+Minh: 0336278037 Support 24/24
+Tele: @minhads14</t>
+        </is>
+      </c>
+      <c r="D623" t="inlineStr">
+        <is>
+          <t>0336278037</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/TPN.NO1</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Trần Phương Nam</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>New
+Lh - zalo: 0333222797</t>
+        </is>
+      </c>
+      <c r="D624" t="inlineStr">
+        <is>
+          <t>0333222797</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61561913071494</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Phi Phung</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>Cung cấp giải pháp Quảng Cáo
+Khoá học chạy Ads
+ZALO: 0355552648</t>
+        </is>
+      </c>
+      <c r="D625" t="inlineStr">
+        <is>
+          <t>0355552648</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/specialhp1</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Minh Tiến</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>Techcombank: 3025.66666666</t>
+        </is>
+      </c>
+      <c r="D626" t="inlineStr">
+        <is>
+          <t>02566666666</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/chuot.be.9465</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Nguyễn Hiếu</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>Chạy Qc Fb, Tiktok, Edit Video, Photoshop
+Tặng FanPage Sẵn 1k Folow
+Contact For Work 034 708 1860</t>
+        </is>
+      </c>
+      <c r="D627" t="inlineStr">
+        <is>
+          <t>0347081860</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vuquangthai111</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Vũ Quang Thái</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>Chạy Quảng cáo ADS - Nguyên liệu
+Call : 039.382.1111</t>
+        </is>
+      </c>
+      <c r="D628" t="inlineStr">
+        <is>
+          <t>0393821111</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100089690417855</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Hiếu Stars</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>メディア
+MEDIA &amp; PRODUCTION AGENCY 0904628088</t>
+        </is>
+      </c>
+      <c r="D629" t="inlineStr">
+        <is>
+          <t>0904628088</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/gayte.vitamin.581</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Bùi Xuân Thịnh</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>ÁP LỰC TẠO LÊN KIM CƯƠNG
+HỖ TRỢ CHẠY ADS FACEBOOK, TIKTOK,......
+CALL; 0586252871</t>
+        </is>
+      </c>
+      <c r="D630" t="inlineStr">
+        <is>
+          <t>0586252871</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/cong.nguyenhoang.39948</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Nguyễn Hoàng Công</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>Chạy &amp; cho thuê tài khoản quảng Cáo
+Zalo: 0567.029.205 - 0363.61.9889
+Tele: @NHC_ADS</t>
+        </is>
+      </c>
+      <c r="D631" t="inlineStr">
+        <is>
+          <t>0567029205, 0363619889</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61562966177112</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Công Hipo</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>HiPo AgenCy
+Chạy &amp; cho thuê tài khoản quảng Cáo
+Zalo: 0567.029.205 - 0363.61.9889
+Tele: @NHC_ADS</t>
+        </is>
+      </c>
+      <c r="D632" t="inlineStr">
+        <is>
+          <t>0567029205, 0363619889</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/hiepop2607</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Trần T. Thanh Hiền</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>HỖ TRỢ DỊCH VỤ MẠNG XÃ HỘI
+TIME:24/24
+SĐT/ZALO:0817586988
+IB CHƯA REP GỌI CHO EM
+DÙNG 1 FB DUY NHẤT</t>
+        </is>
+      </c>
+      <c r="D633" t="inlineStr">
+        <is>
+          <t>0817586988</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vieclammienbac247</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Tuyển Công Nhân Nhà Máy</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>👷🏻‍♂️Tuyển Công Nhân nhà máy, Bao Ăn Ở KTX, Lương thưởng đầy đủ, KoPhí-ko giữ gtờ. ☎️0866.129.766☎️</t>
+        </is>
+      </c>
+      <c r="D634" t="inlineStr">
+        <is>
+          <t>0866129766</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100083622717603</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Vinh Phuc Khuc</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>Zalo : 0787117114
+Twitter : tanquantriston8431</t>
+        </is>
+      </c>
+      <c r="D635" t="inlineStr">
+        <is>
+          <t>0787117114</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100048804002622</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Phát Đạt</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>Chuyên đổ buôn đồ gia dụng, hàng hottrend theo mùa,nhận order hàng trung giá tốt
+Call 0386652866</t>
+        </is>
+      </c>
+      <c r="D636" t="inlineStr">
+        <is>
+          <t>0386652866</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/buon.tatoi.75</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Đểu</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>🏦MB: 0346.555.092 - Lê Vạn Chương</t>
+        </is>
+      </c>
+      <c r="D637" t="inlineStr">
+        <is>
+          <t>0346555092</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61562499507260</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Đỗ Quốc Thịnh</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>Mở khoá Fb.Tăng Follow.Chạy Quảng Cáo Cân VPCS
+☑️Tele: @Thinh Ads
+☎️ Zalo : 0797.234.879(Thịnh Ads)</t>
+        </is>
+      </c>
+      <c r="D638" t="inlineStr">
+        <is>
+          <t>0797234879</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/namnguyenalex</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Nam Nguyễn Alex</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>Cung cấp dịch vụ làm web và tài khoản bán hàng online ở thị trường Âu Mỹ - Liên hệ Zalo 0979923790</t>
+        </is>
+      </c>
+      <c r="D639" t="inlineStr">
+        <is>
+          <t>0979923790</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/Ducnguyen.nets</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Đức Nguyễn</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>𝐇𝐨̂̃ 𝐓𝐫𝐨̛̣ 𝐐𝐮𝐚̉𝐧𝐠 𝐂𝐚́𝐨 𝐅𝐚𝐜𝐞𝐛𝐨𝐨𝐤
+📱0766.93.2222
+📱0767.93.2222</t>
+        </is>
+      </c>
+      <c r="D640" t="inlineStr">
+        <is>
+          <t>0766932222, 0767932222</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/cong.huong.142</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Vương Công Thị Hương</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>Dịch Vụ Digital Marketing
+Liên hệ: 094.558.6363</t>
+        </is>
+      </c>
+      <c r="D641" t="inlineStr">
+        <is>
+          <t>0945586363</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100036099710959</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Văn Trung</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>Hỗ Trợ Dịch Vụ Facebook - Tiktok -ADS Đa Nền Tảng
+Liên Hệ ZaLo : http://Zalo.me/0523929699</t>
+        </is>
+      </c>
+      <c r="D642" t="inlineStr">
+        <is>
+          <t>0523929699</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61559948011709</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Phần Mềm Đăng Bài Tự Động MKT</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>✨Tư vấn xây dựng hệ thống bán hàng đa kênh trên nền tảng MXH✨
+☎️ Contact: 0378179345</t>
+        </is>
+      </c>
+      <c r="D643" t="inlineStr">
+        <is>
+          <t>0378179345</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100048742243746</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Nguyễn Vũ</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>Cty truyền thông HTT99
+Nhận học viên ads
+Nhận chạy quảng cáo fb ,tik tok .
+Liên hệ zalo 0869546221</t>
+        </is>
+      </c>
+      <c r="D644" t="inlineStr">
+        <is>
+          <t>0869546221</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/quanghuong29121990</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Quang Hướng</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>📲 HOTLINE : 0393.150.999
+ATM:MB-2666888399999</t>
+        </is>
+      </c>
+      <c r="D645" t="inlineStr">
+        <is>
+          <t>0393150999</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mannhi2908</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Hữu Đức</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>Sỉ &amp; lẻ dụng cụ rửa xe , xà bông , nhớt , phụ gia cho xe máy 🧽
+💳 Vcb : HUUDUC0808
+☎️ : 0857249943</t>
+        </is>
+      </c>
+      <c r="D646" t="inlineStr">
+        <is>
+          <t>0857249943</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100092242737921</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Nguyễn Văn Bình</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>Sẵn các loại scan và Tktt 1k, rate 45%
+Bao camp bao refund 48h
+Giao dịch trung gian
+LH zalo0978377523</t>
+        </is>
+      </c>
+      <c r="D647" t="inlineStr">
+        <is>
+          <t>0978377523</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/ghenhuaducvuanh</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Bim Bim</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>ghế nhựa đúc Vũ Anh
+Liên hệ qua page hoặc số điện thoại : 0879243688</t>
+        </is>
+      </c>
+      <c r="D648" t="inlineStr">
+        <is>
+          <t>0879243688</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/supportfacebooker3</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Trần Thành Đạt</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>Hỗ trợ &amp; xử lí các vấn đề về Facebook
+Công việc nhắn tin qua Zalo 0827642222 0836378910 . Time 8g-0g⏱</t>
+        </is>
+      </c>
+      <c r="D649" t="inlineStr">
+        <is>
+          <t>08276422220</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/tieu.hoa.5817</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Lê Thị Thanh Hoa</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>NHÀ PHÂN PHỐI 😙SỈ LẺ MỸ PHẨM THÁI LAN HÀNG CHÍNH HÃNG.
+☎️ 0987300008</t>
+        </is>
+      </c>
+      <c r="D650" t="inlineStr">
+        <is>
+          <t>0987300008</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100080468117578</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Lê Kim Thảo</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>♥️ 🍀 Nhận Làm Bùa ❤️ Bùa Làm Ăn🍀Bùa Đồng giới 📌Bùa | DầuHồly- Nước Hoa Phép ❤️Nghành
+📞 0968081241</t>
+        </is>
+      </c>
+      <c r="D651" t="inlineStr">
+        <is>
+          <t>0968081241</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100086088473396</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>My Hipo</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>HIPO AGENCY
+CHẠY &amp; CHO THUÊ TÀI KHOẢN QUẢNG CÁO
+ZALO: 0567029187</t>
+        </is>
+      </c>
+      <c r="D652" t="inlineStr">
+        <is>
+          <t>0567029187</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/luongngoclong.ads</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Lương Ngọc Long</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>Coach Facebook, Tiktok, Google
+☆CHẠY QUẢNG CÁO MỌI LĨNH VỰC ☆
+Call 0965 69 68 92</t>
+        </is>
+      </c>
+      <c r="D653" t="inlineStr">
+        <is>
+          <t>0965696892</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/nguoiconxuhue2011</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Nguyễn Đức</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>"Sự cẩu thả trong bất cứ nghề gì cũng là một sự bất lương."
+Call/ zalo : 0707 26 5555</t>
+        </is>
+      </c>
+      <c r="D654" t="inlineStr">
+        <is>
+          <t>0707265555</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61550678134251</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Nguyễn Diệu Hoa</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>Vận chuyển Trung - Việt và ĐNA.
+Cung cấp dịch vụ Fulfillment ĐNA
+📱0911633035 - Diệu Hoa</t>
+        </is>
+      </c>
+      <c r="D655" t="inlineStr">
+        <is>
+          <t>0911633035</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100033554591644</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Hiệp</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>COMBACK🍀
+Hotline: 0832359876
+0912501113</t>
+        </is>
+      </c>
+      <c r="D656" t="inlineStr">
+        <is>
+          <t>08323598760</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61557674472304</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Cẩm Tú</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>ACE EXPRESS
+Việt 🛫 Mỹ, Úc, Anh, Eu, Malay, Philip, Hàn
+NHANH CHÓNG - UY TÍN - AN TOÀN
+0775536845</t>
+        </is>
+      </c>
+      <c r="D657" t="inlineStr">
+        <is>
+          <t>0775536845</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/leduy.nguyen.100</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Lê Duy Nguyên</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>Zalo 0349.318.616
+Quảng cáo fb/gg/tiktok - Cho thuê tk bm 5%
+Bán Via - Bm - TKQC</t>
+        </is>
+      </c>
+      <c r="D658" t="inlineStr">
+        <is>
+          <t>0349318616</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100093009923168</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Phạm Ngân</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>CANVA PRO VĨNH VIỄN🌿
+Liên hệ Zalo 0918858870 cho nhanh nhé :*</t>
+        </is>
+      </c>
+      <c r="D659" t="inlineStr">
+        <is>
+          <t>0918858870</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100034579084257</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>An Nguyen Car</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>Private car rental service.Sai Gon- Vung Tau-Mui Ne-Can Tho-Airport -Vice versa. Zalo: 0979935944.</t>
+        </is>
+      </c>
+      <c r="D660" t="inlineStr">
+        <is>
+          <t>0979935944</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100091743956691</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Tổng Kho Phụ Tùng Xe Máy Giá Rẻ-Chất Lượng</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>ĐứcAnh company-Nhà phân phối phụ tùng xe máy giá sỉ-lẻ cho toàn thể đại lí-zalo 0979489443</t>
+        </is>
+      </c>
+      <c r="D661" t="inlineStr">
+        <is>
+          <t>0979489443</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100095299104575</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Trần Ái Minh</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>Bán Tk 5m8 - Share link bao cam
+Chiết Khấu Meta - Voi Zalo 0833244246
+https://zalo.me/g/bkocrd827</t>
+        </is>
+      </c>
+      <c r="D662" t="inlineStr">
+        <is>
+          <t>0833244246</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/anlexus12</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Tuân An</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>Xe điện ebikevn.com
+096 8291122</t>
+        </is>
+      </c>
+      <c r="D663" t="inlineStr">
+        <is>
+          <t>0968291122</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/truchuong.tran.566</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Trúc Hương</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>🌵Phun xăm thẩm mỹ 💋🍀
+📞0968130465 😉</t>
+        </is>
+      </c>
+      <c r="D664" t="inlineStr">
+        <is>
+          <t>0968130465</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100055018625282</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Nguyễn Nhi</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>TVT. MB : 08122006260107</t>
+        </is>
+      </c>
+      <c r="D665" t="inlineStr">
+        <is>
+          <t>08122006260</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/langocnguyen109</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>La Ngọc Nguyên</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>STK Mb Bank: 0945690650</t>
+        </is>
+      </c>
+      <c r="D666" t="inlineStr">
+        <is>
+          <t>0945690650</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/nnguyentruong</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Trưởng</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>Chiết khấu Voi,Scan,Tài Nguyên Vip
+Zalo: 038.362.4806
+VCB: 0011004338729
+https://zalo.me/g/momafx494</t>
+        </is>
+      </c>
+      <c r="D667" t="inlineStr">
+        <is>
+          <t>0383624806, 00110043387</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100009418564146</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Công Đức</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>TUYỂN NHÀ PHÂN PHỐI - ĐẠI LÝ BÁNH TRUNG THU TOÀN QUỐC
+https://zalo.me/g/jexhur739
+Zalo: 0867969896</t>
+        </is>
+      </c>
+      <c r="D668" t="inlineStr">
+        <is>
+          <t>0867969896</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100010924001571</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Thìn Đức Nguyễn</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>[I saw you happy without me so i left you!]
+🔥🔥🔥hotline:🔥🔥🔥
+🐉🐉🐉0345.8686.29🐉 🐉🐉</t>
+        </is>
+      </c>
+      <c r="D669" t="inlineStr">
+        <is>
+          <t>0345868629</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100044017937385</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Văn Hoàng</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>Quảng Cáo Fanpage - Tăng Đơn Hàng
+Xây dựng Tik tok
+☎️ Zalo : 0395303798
+Giao Dịch Trung Gian - TT</t>
+        </is>
+      </c>
+      <c r="D670" t="inlineStr">
+        <is>
+          <t>0395303798</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100087426346783</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Nguyễn Diệu Linh</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>Freelancer Marketing/ Design
+Founder Tk Premium
+😼Zalo: 0913383603
+Nguyendieulinh04022003@gmail.com</t>
+        </is>
+      </c>
+      <c r="D671" t="inlineStr">
+        <is>
+          <t>0913383603</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100069912293266</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Đỗ P.Mai</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>Vận chuyển Trung 🛫 ĐNA &amp; Chuyển đổi ngoại tệ.
+UY TÍN - NHIỆT TÌNH - CHẤT LƯỢNG
+☎️ ZALO 0865710526</t>
+        </is>
+      </c>
+      <c r="D672" t="inlineStr">
+        <is>
+          <t>0865710526</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/nguyenquoc97</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Nguyễn Quốc</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>Liên tục tìm đối tác bán hàng về: Hạt dinh dưỡng,v.v...
+SĐT/STK: 0345.886.086 (Nam Á Bank)</t>
+        </is>
+      </c>
+      <c r="D673" t="inlineStr">
+        <is>
+          <t>0345886086</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100014196844271</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Tùng</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>Dịch vụ Facebook(Marketing)
+Nhận Chạy Quảng Cáo Facebook
+Zalo: 0375782743
+Tele: @ads203</t>
+        </is>
+      </c>
+      <c r="D674" t="inlineStr">
+        <is>
+          <t>0375782743</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/thanhthuy932015</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Nguyễn Thanh Thuỷ</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>🛡 👗CHUYÊN THỜI TRANG QUẦN ÁO &amp; TÚI XÁCH
+💎 Liên hệ : 0906790268 💎
+10/722 NGÔ GIA TỰ - HẢI PHÒNG</t>
+        </is>
+      </c>
+      <c r="D675" t="inlineStr">
+        <is>
+          <t>0906790268</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/tienducistore</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Nguyễn Tiến Đức</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>𝙏𝙞ế𝙣 Đứ𝙘 𝙄𝙨𝙩𝙤𝙧𝙚-𝙊𝙣𝙡𝙮 𝘼𝙥𝙥𝙡𝙚  ☎️𝙃𝙤𝙩𝙡𝙞𝙣𝙚: 082.551.6789🏛Trả Góp IPhone 18+</t>
+        </is>
+      </c>
+      <c r="D676" t="inlineStr">
+        <is>
+          <t>0825516789</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100045375822104</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Huyền Quốc Tế</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>Viettel post nhận gửi hàng trong và ngoài nước.
+Liên hệ: 0898105028</t>
+        </is>
+      </c>
+      <c r="D677" t="inlineStr">
+        <is>
+          <t>0898105028</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100077270649242</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Mạnh Tùng</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>VPS US-VN-SIN-EU chính hãng
+Zalo: 0327118632
+Telegram: @Tung24h</t>
+        </is>
+      </c>
+      <c r="D678" t="inlineStr">
+        <is>
+          <t>0327118632</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100075475730669</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Lê Khả Xuân</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>Hỗ trợ ae 24/7 ( Zalo chính : 0833774333 )
+Hệ Thống Bán Hàng Tự Động
+VIAVIP24H.COM</t>
+        </is>
+      </c>
+      <c r="D679" t="inlineStr">
+        <is>
+          <t>0833774333</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/nhungxg68</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Ngọc Quỳnh</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>Chuyên tài khoản Netflix, YT Premium,...
+Cho thuê tài khoản quảng cáo Facebook
+Zalo: 0559 598 120</t>
+        </is>
+      </c>
+      <c r="D680" t="inlineStr">
+        <is>
+          <t>0559598120</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/gucci.huong.520</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Hương Nguyễn</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>Tổng kho Nlm
+Zalo: 0382315539
+Supportads24/7
+CÂN MỌI TRUNG GIAN</t>
+        </is>
+      </c>
+      <c r="D681" t="inlineStr">
+        <is>
+          <t>0382315539</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/nguyendong.mmo</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Nguyễn Văn Đông</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>Tư Vấn Hỗ Trợ Dịch Vụ FB ADS
+Cung cấp Sll nguyên liệu chạy ADS
+🌐 ☎ 09236.01234 ☎️ 0896644999</t>
+        </is>
+      </c>
+      <c r="D682" t="inlineStr">
+        <is>
+          <t>0923601234, 0896644999</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/Vietvpsproxyy</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Tony Việt</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>VPS US-VN-SIN-EU chính hãng
+Zalo: 0983062840
+Telegram:@Pviet_vps
+HOAN HỈ - UY TÍN</t>
+        </is>
+      </c>
+      <c r="D683" t="inlineStr">
+        <is>
+          <t>0983062840</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/lam.m.hoang</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Lâm Minh Hoàng</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>Dịch Vụ Tăng Like Tất Cả Mạng Xã Hội Uy Tín Nhất Tại Cà Mau : Liên Hệ 0706594495.</t>
+        </is>
+      </c>
+      <c r="D684" t="inlineStr">
+        <is>
+          <t>0706594495</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vophummo</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Võ Phú</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>XỬ LÝ MỌI VẤN ĐỀ VỀ MẠNG XÃ HỘI
+Hotline/Zalo: 0787.342.444
+Tele: @Kbich24</t>
+        </is>
+      </c>
+      <c r="D685" t="inlineStr">
+        <is>
+          <t>0787342444</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61558429718513</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Nguyễn Bá Quang</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>CHẠY QUẢNG CÁO MESS + CĐ..vv
+Liên hệ SĐT và ZALO:
+0886.113.989</t>
+        </is>
+      </c>
+      <c r="D686" t="inlineStr">
+        <is>
+          <t>0886113989</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/NGUYENTHANHTHAIHD</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Nguyễn Thành Thái HD</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>CHIẾN LƯỢC TRUYỀN THÔNG DOANH NGHỆP MARKETING QUẢNG CÁO ĐA PHƯƠNG TIỆN 0328 566 188</t>
+        </is>
+      </c>
+      <c r="D687" t="inlineStr">
+        <is>
+          <t>0328566188</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/nguyenthai2611</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Nguyễn Thái</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>Nguyên liệu FB ADS
+call/zalo:0379173326</t>
+        </is>
+      </c>
+      <c r="D688" t="inlineStr">
+        <is>
+          <t>0379173326</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/@tuan838679/</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Nguyễn Thanh Tuấn</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>CHO THUÊ TKQC+CHIẾT KHẤU,SCAN , BUFF FLOW , LIKE PAGE BÀI VIẾT, TĂNG MẮT XEM LIVESTREAM☎ 0969559596</t>
+        </is>
+      </c>
+      <c r="D689" t="inlineStr">
+        <is>
+          <t>0969559596</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/anvy.nguyen.52056</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Nguyễn Quỳnh</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>Chuyên Order - Vận chuyển - OEM
+TQ ➡️ ĐNA
+📲0372.819.654</t>
+        </is>
+      </c>
+      <c r="D690" t="inlineStr">
+        <is>
+          <t>0372819654</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/fc.tanninh</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Mai Tùng Nam</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>CHẠY QUẢNG CÁO LIVE - CUNG CẤP FAN PAGE - HỖ TRỢ XỬ LÝ FB - ☎ 0904829345 - STK_MB 119997899999</t>
+        </is>
+      </c>
+      <c r="D691" t="inlineStr">
+        <is>
+          <t>0904829345</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/sybui2712000</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Bùi Sỹ</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>Hỗ trợ Quảng Cáo Facebook
+SĐT: 0368 307 839
+MB: 9999999 83 8888
+TCB: 9551 6331 888888</t>
+        </is>
+      </c>
+      <c r="D692" t="inlineStr">
+        <is>
+          <t>0368307839</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/huong.nho.52</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Hương Lê</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>Lh cv ib ZALO:0869163416</t>
+        </is>
+      </c>
+      <c r="D693" t="inlineStr">
+        <is>
+          <t>0869163416</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100049346571081</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Nguyễn Hoài</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>📌 Hơn nhau ở chất lượng.🧴📞0345255516</t>
+        </is>
+      </c>
+      <c r="D694" t="inlineStr">
+        <is>
+          <t>0345255516</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100046832783402</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Vinh Quang</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>Cung cấp DV
+sản xuất và quay dựng edit video đa nền tảng
+SPARKSTARSPRODUCTION 093617 5701 -0904628088</t>
+        </is>
+      </c>
+      <c r="D695" t="inlineStr">
+        <is>
+          <t>0936175701, 0904628088</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/hoangnam88886</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Lý Hoàng Nam</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>Chuyên chạy qc ck voi-scan
+📲 0968947136</t>
+        </is>
+      </c>
+      <c r="D696" t="inlineStr">
+        <is>
+          <t>0968947136</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100007790830836</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Đặng Minh Tú</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>Nhận chụp Phóng Sự Cưới ABC mọi thể loại
+Hotline:0877992922
+STK : MB BANK
+0877992922 - DANG MINH TU</t>
+        </is>
+      </c>
+      <c r="D697" t="inlineStr">
+        <is>
+          <t>0877992922, 0877992922</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mduy2808</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Hà Minh Duy</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>🔊 XỬ LÝ MỌI VẤN ĐỀ VỀ MẠNG XÃ HỘI
+👇
+📲Hotline/Zalo: 0388.2808.07 ☎️
+Telegram : t.me/hmdshop2808</t>
+        </is>
+      </c>
+      <c r="D698" t="inlineStr">
+        <is>
+          <t>0388280807</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61558730091285</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Kim Ngân</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>SPX Express - Ngoài sàn Shopee
+Đồng giá toàn quốc chỉ từ 12k/đơn
+Inbox/zalo 0915.145.233 để tư vấn ạ!</t>
+        </is>
+      </c>
+      <c r="D699" t="inlineStr">
+        <is>
+          <t>0915145233</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100084156377502</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Phan Văn Trung</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>Cung cấp VPS-Proxy chính hãng
+-
+1036940266
+PHAN VAN TRUNG
+VIETCOMBANK
+-
+Zalo: 0967834290</t>
+        </is>
+      </c>
+      <c r="D700" t="inlineStr">
+        <is>
+          <t>0967834290</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/than.but.129</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Như Hoa</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>- Chuyên Cung cấp Thiết Bị Vệ Sinh PORO / Gạch đá ốp lát / Vật tư xây dựng / Hotline : 0911896986</t>
+        </is>
+      </c>
+      <c r="D701" t="inlineStr">
+        <is>
+          <t>0911896986</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100043661783706</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Nguyễn Tuyết Ngân</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>PHUN XĂM THẨM MỸ 🌸
+Booking : 0384941240</t>
+        </is>
+      </c>
+      <c r="D702" t="inlineStr">
+        <is>
+          <t>0384941240</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61553160114622</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Nuywen Chi</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>💥Chiết Khấu | VOI - Scan - TUT - Ngưỡng...
+📌Cung Cấp TKQC - Cân all VPCS❗
+🔰Call/Zalo : 0987043206✅</t>
+        </is>
+      </c>
+      <c r="D703" t="inlineStr">
+        <is>
+          <t>0987043206</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100064590672232</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Hà Mai Châu</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>Sỉ/lẻ gia dụng gia đình, âm thanh, thiết bị vệ sinh,vật tư điện nước,...
+LH: 0917963322 ( có zalo )</t>
+        </is>
+      </c>
+      <c r="D704" t="inlineStr">
+        <is>
+          <t>0917963322</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/phihung.nguyenhuu.06</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Nguyen Huu Phi Hung</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>Minh Hòa ❤️
+Facebook ads A-Z
+☎️ 0394554408
+Tele: phihungads01</t>
+        </is>
+      </c>
+      <c r="D705" t="inlineStr">
+        <is>
+          <t>0394554408</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/th.chuotbaby</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Dương Tấn Hậu</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>#KIENTRI
+#NOLUC
+#TIETKIEM
+#THANHCONG
+Call: 0338.469.239 📞📞</t>
+        </is>
+      </c>
+      <c r="D706" t="inlineStr">
+        <is>
+          <t>0338469239</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100024268180265</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Đặng Hà Giang</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>đây ACC phụ xin liên hệ đến
+📞 Tele: @danghagiang
+✴️ Zalo : 0368441631</t>
+        </is>
+      </c>
+      <c r="D707" t="inlineStr">
+        <is>
+          <t>0368441631</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/huumanhmarketing</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Nguyễn Hữu Mạnh</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>🔷ChạyQC FB,Zalo🔷
+🍀Liên hệ: 0865448695🍀
+🍁Cho thuê Group🍁
+🍁NGUYEN HUU MANH🍁</t>
+        </is>
+      </c>
+      <c r="D708" t="inlineStr">
+        <is>
+          <t>0865448695</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100041819892599</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Nhật HằngSpa</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>❤CHUYÊN ĐIỀU TRỊ:MỤN-NÁM-TÀN NHANG-SẸO RỖ-HÔI NÁCH-DA BỊ NHIỄM CHÌ❤👉STK 30101711999999👈0387141325💦</t>
+        </is>
+      </c>
+      <c r="D709" t="inlineStr">
+        <is>
+          <t>01017119999, 0387141325</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/Ducfacebook90</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Nguyễn Văn Đức</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>💎Hỗ trợ Mạng Xã Hội💎FACEBOOK-TIKTOK ☎️0961.275.240 ✅ Dich Vụ Tăng tương tác - Mở khoá Facebook 🔓</t>
+        </is>
+      </c>
+      <c r="D710" t="inlineStr">
+        <is>
+          <t>0961275240</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100047962750456</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Nguyễn Đông</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>CHÚC MỪNG KHÁCH HÀNG DÀNH CHIẾN THẮNG
+LH Zalo : 0832.00.9999
+Hotline : 0832.00.9999</t>
+        </is>
+      </c>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t>0832009999, 0832009999</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/duongducanh123</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Dương Đức Anh</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>Content - Thiết kế - Chăm sóc Fanpage - Facebook Ads
+📲 0938229592</t>
+        </is>
+      </c>
+      <c r="D712" t="inlineStr">
+        <is>
+          <t>0938229592</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100024683674177</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Bình Nguyễn</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>Thiết Kế Social Media, Facebook Ads, Tik Tok Ads Thiết kế Website LH: 0795661737</t>
+        </is>
+      </c>
+      <c r="D713" t="inlineStr">
+        <is>
+          <t>0795661737</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/bameo.vn</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Nguyễn Mạnh Hiếu</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>Tích Xanh | Quảng Cáo | Tương Tác | Mở Khóa
+☎ Hotline : 0345.150.999
+📱 Zalo : 0976.116.805</t>
+        </is>
+      </c>
+      <c r="D714" t="inlineStr">
+        <is>
+          <t>0345150999, 0976116805</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100080417119867</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Trường Stars</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>Thiết kế / Edit video ( Graphic motion/ TVC/ Animation) - Video đa nền tảng - 090 4628088</t>
+        </is>
+      </c>
+      <c r="D715" t="inlineStr">
+        <is>
+          <t>0904628088</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61562836021927</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Nguyễn Đồng</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>🔥Chuyên cung cấp nguyên liệu ADS🔥
+👉uy tín - chất lượng✅
+VIETINBANK STK: 108881021175</t>
+        </is>
+      </c>
+      <c r="D716" t="inlineStr">
+        <is>
+          <t>08881021175</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/lethithuthuy.2109</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Lê Thị Thu Thuỷ</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>THU THUỶ SPORTS - Chuyên sỉ lẻ &amp; in ấn quần áo bóng đá, đồng phục. Liên hệ: 0342.688.227</t>
+        </is>
+      </c>
+      <c r="D717" t="inlineStr">
+        <is>
+          <t>0342688227</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100045151186234</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Kiên Trung</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>Phân phối nội thất ô tô ☎Zalo 0968826538</t>
+        </is>
+      </c>
+      <c r="D718" t="inlineStr">
+        <is>
+          <t>0968826538</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/hao5stpro</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Đỗ Anh Hào</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>Hổ trợ Facebook - instagram - Tiktok - Youtube - Google
+Zalo Contact 0394438852</t>
+        </is>
+      </c>
+      <c r="D719" t="inlineStr">
+        <is>
+          <t>0394438852</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/ut.muoi.31</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Lê Hương</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>VIETCOM : 1015722678
+VIETTIN : 104877273393
+BIDV : 8883087532
+☎️ 0️⃣9️⃣6️⃣2️⃣6️⃣4️⃣8️⃣7️⃣0️⃣8️⃣</t>
+        </is>
+      </c>
+      <c r="D720" t="inlineStr">
+        <is>
+          <t>04877273393</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vanlangdulich</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Văn Lăng</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>Tour Sapa - Hà Giang - Y Tý | Trekking | Hiking | Tour Trung Quốc | FB ADS |
+📞 083 7979 883 ( Zalo )</t>
+        </is>
+      </c>
+      <c r="D721" t="inlineStr">
+        <is>
+          <t>0837979883</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/kimquyen304</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Kim Quyên</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>LIÊN HỆ CÔNG VIỆC: 0353.041.240</t>
+        </is>
+      </c>
+      <c r="D722" t="inlineStr">
+        <is>
+          <t>0353041240</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/lequyfanpage26</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Lê Quý</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>Mua Bán FanPage
+Hỗ trợ &amp; xử lý mọi vấn đề về Facebook-Instargram-TikTok
+Contact/Zalo :☎️086.549.4473</t>
+        </is>
+      </c>
+      <c r="D723" t="inlineStr">
+        <is>
+          <t>0865494473</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/tranvanphongmedia</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Trần Văn Phong</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>☆ Online Marketing Services ☆🔥
+⚔️ Xử Lý Mọi Vấn Đề Về MXH⚔️
+📲 Contact/Zalo: 0395534287 ☎</t>
+        </is>
+      </c>
+      <c r="D724" t="inlineStr">
+        <is>
+          <t>0395534287</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/hiep.ngo.142</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Hiep Ngo</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>Xưởng SX Vòng Tay Tràng Hạt Gỗ Giá rẻ
+call - 08.3534.9999
+zalo sỉ - 0358.993.999 - 0333.303.222</t>
+        </is>
+      </c>
+      <c r="D725" t="inlineStr">
+        <is>
+          <t>0835349999, 0358993999, 0333303222</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/chauloanorder</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Loan Trần</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>Liên hệ: 0343213826 (imess/zalo/call)</t>
+        </is>
+      </c>
+      <c r="D726" t="inlineStr">
+        <is>
+          <t>0343213826</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61553609505425</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Nguyễn Trung Hiếu</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>Chuyên cung cấp các dong xe Mg
+Uy Tín-nhiệt Tình-Tận Tâm
+0975.590.675</t>
+        </is>
+      </c>
+      <c r="D727" t="inlineStr">
+        <is>
+          <t>0975590675</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100003709060156</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Nguyễn Phong</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>Quiri Hotel &amp; Restaurant | Qui’s Homestay |Quiri Peninsula Hostel | Ha Giang Vision Tour +84981623096</t>
+        </is>
+      </c>
+      <c r="D728" t="inlineStr">
+        <is>
+          <t>0981623096</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/huanmmo21</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Huân Đinh Văn</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>Zalo/Phone : 0345.051.868 - 052.203.1234 🇻🇳
+Tele : @huandinhvan102</t>
+        </is>
+      </c>
+      <c r="D729" t="inlineStr">
+        <is>
+          <t>0345051868, 0522031234</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/UYTINCHATLUONGCAO99</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Lê Nhật Tân - Cung Cấp Fanpage - Liên Hệ Zalo 085 888 1722</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>Mua Bán Fanpage
+Hỗ trợ &amp; xử lý mọi vấn đề về Facebook-Instargram-TikTok
+Gọi/Zalo : ☎️085.888.1722
+-</t>
+        </is>
+      </c>
+      <c r="D730" t="inlineStr">
+        <is>
+          <t>0858881722</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100009421007282</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Huyền Lì</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>𝐌𝐄𝐘𝐌𝐀𝐊𝐄𝐔𝐏 𝐒𝐓𝐎𝐑𝐄-0969535590
+📍: 𝟔𝟏𝟔 𝐋𝐞 𝐃𝐮𝐚𝐧-𝐓𝐩 𝐒𝐨𝐧 𝐋𝐚</t>
+        </is>
+      </c>
+      <c r="D731" t="inlineStr">
+        <is>
+          <t>0969535590</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100076889481355</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Kho Sỉ Anh Châu</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>Oder -Vận chuyển Trung Việt Lào Cam
+ZAL: 0522225888</t>
+        </is>
+      </c>
+      <c r="D732" t="inlineStr">
+        <is>
+          <t>0522225888</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/hoa.duongthi.39904181</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Dương Thị Hoa</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>Làm điều mình muốn
+Biến ước mơ thành hiện thực 💃💃💃
+ZALO :0985465168</t>
+        </is>
+      </c>
+      <c r="D733" t="inlineStr">
+        <is>
+          <t>0985465168</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100015184518155</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Khương Khánh Duy</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>Nhà đất nền Hà Nội nguyên căn chỉ từ 2 - 3 tỉ đã có nhà - Tư vấn miễn phí và xem nhà - 036.3909.423</t>
+        </is>
+      </c>
+      <c r="D734" t="inlineStr">
+        <is>
+          <t>0363909423</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/Nguyentanlong.Mmo</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Nguyễn Tấn Long</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>SUPPORT FACEBOOK - INSTGRAM - TIK TOK
+DỊCH VỤ TÍCH XANH
+Zalo/Call : 03529.112.91
+Tele:Mrlonginfo3979</t>
+        </is>
+      </c>
+      <c r="D735" t="inlineStr">
+        <is>
+          <t>0352911291</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/ceoleducanh</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Lê Đức Anh</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>👉Xưởng Sản Xuất Vòng Tay Tỳ Hưu 10 Ly👈
+HOTLINE: 096.910.6829
+VIB: 865.99.6666
+MB: 668.666.888.6666</t>
+        </is>
+      </c>
+      <c r="D736" t="inlineStr">
+        <is>
+          <t>0969106829</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/tamtatvn</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Tâm Tất</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>Chuyên sỉ lẻ tất vớ link tham gia nhóm https://zalo.me/g/sabthl825
+sđt zalo: 0328 772 918</t>
+        </is>
+      </c>
+      <c r="D737" t="inlineStr">
+        <is>
+          <t>0328772918</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/uyen.nhi.77128261</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Uyển Nhi</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>Chuyên gia dụng + mỹ phẩm hàng nhập khẩu !
+💰MB : 0899989469- Lê Thị Diệu Huyền
+📱08.999.89.369</t>
+        </is>
+      </c>
+      <c r="D738" t="inlineStr">
+        <is>
+          <t>0899989469, 0899989369</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100069121610020</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Nguyen Huyen Trangg</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>Khám, Chữa Gian Hàng Shopee
+Xây Dựng + Vận Hành + Chạy ADS ra đơn
+📞 0972.127.813</t>
+        </is>
+      </c>
+      <c r="D739" t="inlineStr">
+        <is>
+          <t>0972127813</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/nghi.viet.733</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Lưu Thanh Bình</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>Chuyên Airpod 🍎 Apple Watch 📲 0356632578</t>
+        </is>
+      </c>
+      <c r="D740" t="inlineStr">
+        <is>
+          <t>0356632578</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100039551213134</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Nguyễn Duy Hoàng</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>Xin Chào &lt;-&gt; Tạm Biệt 🤍
+0971053914</t>
+        </is>
+      </c>
+      <c r="D741" t="inlineStr">
+        <is>
+          <t>0971053914</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vutuananh19900</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Anh Vũ</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>Chạy quảng cáo live stream cho 300 shop từ Bắc vào Nam
+Zalo công việc:
+📲098703.9999 0911.333.777</t>
+        </is>
+      </c>
+      <c r="D742" t="inlineStr">
+        <is>
+          <t>09870399990</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/sieumong.145</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Đỗ Thanh Trình</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>MUA BÁN FANPAGE
+CHẠY QUẢNG CÁO FACEBOOK
+CALL/ZALO 087.638.5555🐯- 0393.013.252🐯</t>
+        </is>
+      </c>
+      <c r="D743" t="inlineStr">
+        <is>
+          <t>0876385555, 0393013252</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100071167779886</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Hương Hipo</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>Hipo Agency
+Cho thuê &amp; chạy quảng cáo
+LH zalo 0568252157</t>
+        </is>
+      </c>
+      <c r="D744" t="inlineStr">
+        <is>
+          <t>0568252157</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/ads.media.2022</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Nam Hoàng</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>CÔNG TY XMedia - Digital Marketing
+📩xmedia@contact-meta.vn
+☎️Call/Zalo: 0876.47.9999 • 0584.82.5678</t>
+        </is>
+      </c>
+      <c r="D745" t="inlineStr">
+        <is>
+          <t>0876479999, 0584825678</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/ninhyen0209</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Ninh Thị Yến</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>𝑺𝑰̉ 𝑳𝑬̉ 𝑮𝑰𝑨̉𝑴 𝑪𝑨̂𝑵 - 𝑪𝑨𝑶 𝑮𝑼̛̀𝑵𝑮 𝑮𝑰𝑨̉𝑴 𝑴𝑶̛̃ - 𝑳𝑨𝑻𝑬𝑿
+𝒁𝑳 : 0971.486.112</t>
+        </is>
+      </c>
+      <c r="D746" t="inlineStr">
+        <is>
+          <t>0971486112</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/longatcer</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Long Hipo</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>HiPo AgenCy
+Chạy &amp; cho thuê tài khoản quảng Cáo
+Zalo: 0568.253.224 - 0877732308
+Tele: @goodnai2222</t>
+        </is>
+      </c>
+      <c r="D747" t="inlineStr">
+        <is>
+          <t>0568253224, 0877732308</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=61562417025570</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Đỗ Thảo Uyên</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>Marketing Online - Academy - Media - Land
+Hotline: 0798615948</t>
+        </is>
+      </c>
+      <c r="D748" t="inlineStr">
+        <is>
+          <t>0798615948</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/Dangnhat.minh86</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Đặng Nhật Minh</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>ㅤSupportㅤ
+𝙁𝘼𝘾𝙀𝘽𝙊𝙊𝙆- 𝙄𝙉𝙎𝙏𝘼𝙂𝙍𝘼𝙈-𝙏𝙞𝙠𝙏𝙤𝙠ㅤ󱙄
+☎️ Zalo.me/0865591149</t>
+        </is>
+      </c>
+      <c r="D749" t="inlineStr">
+        <is>
+          <t>0865591149</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/nmh.n072002</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Nguyễn Mạnh Hùng</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>Tư Vấn Căn Hộ Chuyển Nhượng Và Cho Thuê
+Sỉ Lẻ Apple Chính Hãng 🍏
+📞 0899.309.789
+Kv : Hà Nội</t>
+        </is>
+      </c>
+      <c r="D750" t="inlineStr">
+        <is>
+          <t>0899309789</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/quytri.nguyen</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Nguyễn Quý Trí</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>👉🏻0938.722.282👈🏻 (for work)</t>
+        </is>
+      </c>
+      <c r="D751" t="inlineStr">
+        <is>
+          <t>0938722282</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/profile.php?id=100014259213618</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Nguyễn Thanh Tâm</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>[ Group 365 ]
+1. Nhận chạy All các app Ngân hàng- Kyc
+2. Liên kết CTV: Tài chính, Nhà mạng
+0386985386</t>
+        </is>
+      </c>
+      <c r="D752" t="inlineStr">
+        <is>
+          <t>0386985386</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/@Dangkhoads/</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Đăng Khoa</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>CUNG CẤP TÀI NGUYÊN
+CHẠY QUẢNG CÁO FACEBOOK
+💎Hợp Tác lâu dài💎
+☎️ Zalo : 0934.841.365✅</t>
+        </is>
+      </c>
+      <c r="D753" t="inlineStr">
+        <is>
+          <t>0934841365</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/phucbonz.9999</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Đào Công Phúc</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>✅NHẬN CHẠY QUẢNG CÁO FACEBOOK
+CUNG CẤP - CHO THUÊ TKQC
+📞Liên Hệ 07.99.05.4444</t>
+        </is>
+      </c>
+      <c r="D754" t="inlineStr">
+        <is>
+          <t>0799054444</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/guihangdimyuccanadataidanang</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Nam Thịnh</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>☘️🍀Nhận gửi hàng đi tất cả các nước.Nhận đa dạng các mặt hàng.📲0835 143 143</t>
+        </is>
+      </c>
+      <c r="D755" t="inlineStr">
+        <is>
+          <t>0835143143</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/bogia.cuong.9</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Trại Ốc Hoàng Cường</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>chuyên cung cấp ốc giống ốc thịt mọi miền tổ quốc.sđt 0795228333. Mb 088816589999</t>
+        </is>
+      </c>
+      <c r="D756" t="inlineStr">
+        <is>
+          <t>0795228333, 08881658999</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/giang.dance.3</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Lê Văn Giang</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>Uy tín làm lên thương hiệu 💸💸
+Liên hệ 24/7 🚀🚀 0354253423 1027573484 vietcom Lê Văn Giang</t>
+        </is>
+      </c>
+      <c r="D757" t="inlineStr">
+        <is>
+          <t>03542534231</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>